<commit_message>
changed numeric values to probs, creates draft for distrib - birads tested OK
</commit_message>
<xml_diff>
--- a/findings/output.xlsx
+++ b/findings/output.xlsx
@@ -1192,25 +1192,25 @@
         <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E2" t="n">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J2" t="s">
         <v>24</v>
@@ -2127,25 +2127,25 @@
         <v>87</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E27" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="F27" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J27" t="s">
         <v>24</v>
@@ -3040,25 +3040,25 @@
         <v>104</v>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D52" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G52" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="H52" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J52" t="s">
         <v>24</v>
@@ -3937,25 +3937,25 @@
         <v>111</v>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G77" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H77" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="I77" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J77" t="s">
         <v>24</v>
@@ -4844,25 +4844,25 @@
         <v>122</v>
       </c>
       <c r="C102" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D102" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E102" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="F102" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G102" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H102" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J102" t="s">
         <v>24</v>
@@ -5743,25 +5743,25 @@
         <v>29</v>
       </c>
       <c r="C127" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D127" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E127" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F127" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G127" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H127" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="I127" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J127" t="s">
         <v>24</v>
@@ -6652,25 +6652,25 @@
         <v>133</v>
       </c>
       <c r="C152" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D152" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E152" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="F152" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G152" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H152" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I152" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J152" t="s">
         <v>24</v>
@@ -7555,25 +7555,25 @@
         <v>137</v>
       </c>
       <c r="C177" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D177" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E177" t="n">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="F177" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G177" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H177" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I177" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J177" t="s">
         <v>24</v>
@@ -8460,25 +8460,25 @@
         <v>142</v>
       </c>
       <c r="C202" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D202" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E202" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F202" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G202" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="H202" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I202" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J202" t="s">
         <v>24</v>
@@ -9371,25 +9371,25 @@
         <v>148</v>
       </c>
       <c r="C227" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D227" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E227" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F227" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G227" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H227" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I227" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J227" t="s">
         <v>24</v>
@@ -10278,25 +10278,25 @@
         <v>154</v>
       </c>
       <c r="C252" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D252" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E252" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F252" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G252" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H252" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I252" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J252" t="s">
         <v>24</v>
@@ -11187,25 +11187,25 @@
         <v>162</v>
       </c>
       <c r="C277" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D277" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E277" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="F277" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="G277" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H277" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I277" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J277" t="s">
         <v>24</v>
@@ -12096,25 +12096,25 @@
         <v>172</v>
       </c>
       <c r="C302" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D302" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E302" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="F302" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G302" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H302" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I302" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J302" t="s">
         <v>24</v>
@@ -13003,25 +13003,25 @@
         <v>175</v>
       </c>
       <c r="C327" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D327" t="n">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="E327" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F327" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G327" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H327" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I327" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J327" t="s">
         <v>24</v>
@@ -13900,25 +13900,25 @@
         <v>177</v>
       </c>
       <c r="C352" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D352" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E352" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F352" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G352" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="H352" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I352" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J352" t="s">
         <v>24</v>
@@ -14829,25 +14829,25 @@
         <v>196</v>
       </c>
       <c r="C377" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D377" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E377" t="n">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="F377" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G377" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="H377" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I377" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J377" t="s">
         <v>24</v>
@@ -15748,25 +15748,25 @@
         <v>200</v>
       </c>
       <c r="C402" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D402" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E402" t="n">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="F402" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="G402" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="H402" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I402" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J402" t="s">
         <v>24</v>
@@ -16667,25 +16667,25 @@
         <v>211</v>
       </c>
       <c r="C427" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D427" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E427" t="n">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="F427" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G427" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H427" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I427" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J427" t="s">
         <v>24</v>
@@ -17576,25 +17576,25 @@
         <v>217</v>
       </c>
       <c r="C452" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D452" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E452" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F452" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G452" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H452" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I452" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J452" t="s">
         <v>24</v>
@@ -18489,25 +18489,25 @@
         <v>223</v>
       </c>
       <c r="C477" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D477" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E477" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F477" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G477" t="n">
-        <v>30</v>
-      </c>
-      <c r="H477" t="s">
-        <v>18</v>
+        <v>0.3</v>
+      </c>
+      <c r="H477" t="n">
+        <v>0.04</v>
       </c>
       <c r="I477" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J477" t="s">
         <v>24</v>
@@ -19396,25 +19396,25 @@
         <v>227</v>
       </c>
       <c r="C502" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D502" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E502" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F502" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G502" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="H502" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I502" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J502" t="s">
         <v>24</v>
@@ -20309,25 +20309,25 @@
         <v>230</v>
       </c>
       <c r="C527" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D527" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E527" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F527" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G527" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="H527" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="I527" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J527" t="s">
         <v>24</v>
@@ -21220,25 +21220,25 @@
         <v>236</v>
       </c>
       <c r="C552" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D552" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E552" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F552" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G552" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="H552" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="I552" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J552" t="s">
         <v>24</v>
@@ -22131,25 +22131,25 @@
         <v>242</v>
       </c>
       <c r="C577" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="D577" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="E577" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="F577" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="G577" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="H577" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="I577" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J577" t="s">
         <v>24</v>

</xml_diff>